<commit_message>
Fix advanced tutorial to add tag
</commit_message>
<xml_diff>
--- a/tutorial/Advanced_Tutorial/advanced.xlsx
+++ b/tutorial/Advanced_Tutorial/advanced.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dgarijo\Documents\GitHub\t2wml\tutorial\Advanced_Tutorial\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="00_advanced" sheetId="1" r:id="rId1"/>
@@ -13,12 +18,12 @@
     <sheet name="03_advanced_exercise" sheetId="4" r:id="rId4"/>
     <sheet name="03_advanced_solution" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="32">
   <si>
     <t>dataset</t>
   </si>
@@ -102,16 +107,36 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>Tutorial dataset title</t>
+  </si>
+  <si>
+    <t>This is a description for the datatest used in the tutorial</t>
+  </si>
+  <si>
+    <t>https://github.com/usc-isi-i2/t2wml/tree/master/tutorial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,17 +159,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -191,7 +227,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -223,9 +259,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -257,6 +294,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -432,22 +470,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -461,7 +510,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -475,96 +524,106 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>13</v>
       </c>
       <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
         <v>18</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>28</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -572,7 +631,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -586,7 +645,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -600,73 +659,78 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="C9" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="B10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>17</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="C11" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
         <v>18</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>28</v>
       </c>
     </row>
@@ -676,14 +740,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -691,7 +757,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -708,7 +774,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -725,120 +791,125 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="D8">
-        <v>2018</v>
-      </c>
-      <c r="E8">
+      <c r="D9">
+        <v>2018</v>
+      </c>
+      <c r="E9">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="D9">
-        <v>2019</v>
-      </c>
-      <c r="E9">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>2019</v>
+      </c>
+      <c r="E10">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="C10" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="D10">
-        <v>2018</v>
-      </c>
-      <c r="E10">
+      <c r="D11">
+        <v>2018</v>
+      </c>
+      <c r="E11">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="D11">
-        <v>2019</v>
-      </c>
-      <c r="E11">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>2019</v>
+      </c>
+      <c r="E12">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="B12" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="D12">
-        <v>2018</v>
-      </c>
-      <c r="E12">
+      <c r="D13">
+        <v>2018</v>
+      </c>
+      <c r="E13">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="D13">
-        <v>2019</v>
-      </c>
-      <c r="E13">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>2019</v>
+      </c>
+      <c r="E14">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="C14" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
         <v>18</v>
       </c>
-      <c r="D14">
-        <v>2018</v>
-      </c>
-      <c r="E14">
+      <c r="D15">
+        <v>2018</v>
+      </c>
+      <c r="E15">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="D15">
-        <v>2019</v>
-      </c>
-      <c r="E15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>2019</v>
+      </c>
+      <c r="E16">
         <v>30</v>
       </c>
     </row>
@@ -848,14 +919,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -863,7 +936,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -883,7 +956,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -903,211 +976,216 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>24</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>26</v>
       </c>
-      <c r="E8">
-        <v>2018</v>
-      </c>
-      <c r="F8">
+      <c r="E9">
+        <v>2018</v>
+      </c>
+      <c r="F9">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="E9">
-        <v>2019</v>
-      </c>
-      <c r="F9">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>2019</v>
+      </c>
+      <c r="F10">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="D10" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
         <v>27</v>
       </c>
-      <c r="E10">
-        <v>2018</v>
-      </c>
-      <c r="F10">
+      <c r="E11">
+        <v>2018</v>
+      </c>
+      <c r="F11">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="E11">
-        <v>2019</v>
-      </c>
-      <c r="F11">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>2019</v>
+      </c>
+      <c r="F12">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="C12" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
         <v>18</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>26</v>
       </c>
-      <c r="E12">
-        <v>2018</v>
-      </c>
-      <c r="F12">
+      <c r="E13">
+        <v>2018</v>
+      </c>
+      <c r="F13">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="E13">
-        <v>2019</v>
-      </c>
-      <c r="F13">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>2019</v>
+      </c>
+      <c r="F14">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="D14" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
         <v>27</v>
       </c>
-      <c r="E14">
-        <v>2018</v>
-      </c>
-      <c r="F14">
+      <c r="E15">
+        <v>2018</v>
+      </c>
+      <c r="F15">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="E15">
-        <v>2019</v>
-      </c>
-      <c r="F15">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>2019</v>
+      </c>
+      <c r="F16">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="B16" t="s">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
         <v>13</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>17</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>26</v>
       </c>
-      <c r="E16">
-        <v>2018</v>
-      </c>
-      <c r="F16">
+      <c r="E17">
+        <v>2018</v>
+      </c>
+      <c r="F17">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="3:6">
-      <c r="E17">
-        <v>2019</v>
-      </c>
-      <c r="F17">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>2019</v>
+      </c>
+      <c r="F18">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="3:6">
-      <c r="D18" t="s">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="E18">
-        <v>2018</v>
-      </c>
-      <c r="F18">
+      <c r="E19">
+        <v>2018</v>
+      </c>
+      <c r="F19">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="3:6">
-      <c r="E19">
-        <v>2019</v>
-      </c>
-      <c r="F19">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>2019</v>
+      </c>
+      <c r="F20">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="3:6">
-      <c r="C20" t="s">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
         <v>18</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>26</v>
       </c>
-      <c r="E20">
-        <v>2018</v>
-      </c>
-      <c r="F20">
+      <c r="E21">
+        <v>2018</v>
+      </c>
+      <c r="F21">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="3:6">
-      <c r="E21">
-        <v>2019</v>
-      </c>
-      <c r="F21">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>2019</v>
+      </c>
+      <c r="F22">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="3:6">
-      <c r="D22" t="s">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
         <v>27</v>
       </c>
-      <c r="E22">
-        <v>2018</v>
-      </c>
-      <c r="F22">
+      <c r="E23">
+        <v>2018</v>
+      </c>
+      <c r="F23">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="3:6">
-      <c r="E23">
-        <v>2019</v>
-      </c>
-      <c r="F23">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>2019</v>
+      </c>
+      <c r="F24">
         <v>31</v>
       </c>
     </row>
@@ -1117,14 +1195,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1132,7 +1212,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1152,7 +1232,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1172,211 +1252,216 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>24</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>26</v>
       </c>
-      <c r="E8">
-        <v>2018</v>
-      </c>
-      <c r="F8">
+      <c r="E9">
+        <v>2018</v>
+      </c>
+      <c r="F9">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="E9">
-        <v>2019</v>
-      </c>
-      <c r="F9">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>2019</v>
+      </c>
+      <c r="F10">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="D10" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
         <v>27</v>
       </c>
-      <c r="E10">
-        <v>2018</v>
-      </c>
-      <c r="F10">
+      <c r="E11">
+        <v>2018</v>
+      </c>
+      <c r="F11">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="E11">
-        <v>2019</v>
-      </c>
-      <c r="F11">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>2019</v>
+      </c>
+      <c r="F12">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="C12" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
         <v>18</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>26</v>
       </c>
-      <c r="E12">
-        <v>2018</v>
-      </c>
-      <c r="F12">
+      <c r="E13">
+        <v>2018</v>
+      </c>
+      <c r="F13">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="E13">
-        <v>2019</v>
-      </c>
-      <c r="F13">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>2019</v>
+      </c>
+      <c r="F14">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="D14" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
         <v>27</v>
       </c>
-      <c r="E14">
-        <v>2018</v>
-      </c>
-      <c r="F14">
+      <c r="E15">
+        <v>2018</v>
+      </c>
+      <c r="F15">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="E15">
-        <v>2019</v>
-      </c>
-      <c r="F15">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>2019</v>
+      </c>
+      <c r="F16">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="B16" t="s">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
         <v>13</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>17</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>26</v>
       </c>
-      <c r="E16">
-        <v>2018</v>
-      </c>
-      <c r="F16">
+      <c r="E17">
+        <v>2018</v>
+      </c>
+      <c r="F17">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="3:6">
-      <c r="E17">
-        <v>2019</v>
-      </c>
-      <c r="F17">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>2019</v>
+      </c>
+      <c r="F18">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="3:6">
-      <c r="D18" t="s">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="E18">
-        <v>2018</v>
-      </c>
-      <c r="F18">
+      <c r="E19">
+        <v>2018</v>
+      </c>
+      <c r="F19">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="3:6">
-      <c r="E19">
-        <v>2019</v>
-      </c>
-      <c r="F19">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>2019</v>
+      </c>
+      <c r="F20">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="3:6">
-      <c r="C20" t="s">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
         <v>18</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>26</v>
       </c>
-      <c r="E20">
-        <v>2018</v>
-      </c>
-      <c r="F20">
+      <c r="E21">
+        <v>2018</v>
+      </c>
+      <c r="F21">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="3:6">
-      <c r="E21">
-        <v>2019</v>
-      </c>
-      <c r="F21">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>2019</v>
+      </c>
+      <c r="F22">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="3:6">
-      <c r="D22" t="s">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
         <v>27</v>
       </c>
-      <c r="E22">
-        <v>2018</v>
-      </c>
-      <c r="F22">
+      <c r="E23">
+        <v>2018</v>
+      </c>
+      <c r="F23">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="3:6">
-      <c r="E23">
-        <v>2019</v>
-      </c>
-      <c r="F23">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>2019</v>
+      </c>
+      <c r="F24">
         <v>31</v>
       </c>
     </row>

</xml_diff>